<commit_message>
Add SQL features and calculate pace
</commit_message>
<xml_diff>
--- a/running.xlsx
+++ b/running.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ishanshah/Documents/Personal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ishanshah/Documents/Programming/Projects/runkeeper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0AEC08-7FAD-D34F-982F-1A3C6745455D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D80C256-9075-C243-BE8F-2500EB32ABAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="1540" windowWidth="28040" windowHeight="17440" xr2:uid="{0359BB1E-FD39-1146-807B-EC4AC9C4810C}"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{0359BB1E-FD39-1146-807B-EC4AC9C4810C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="main" sheetId="1" r:id="rId1"/>
+    <sheet name="test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -41,9 +42,6 @@
     <t>Pace (min/mi)</t>
   </si>
   <si>
-    <t>Time (min)</t>
-  </si>
-  <si>
     <t>Split 1</t>
   </si>
   <si>
@@ -161,9 +159,6 @@
     <t>11:56</t>
   </si>
   <si>
-    <t>Total Distance (mi)</t>
-  </si>
-  <si>
     <t>22:36</t>
   </si>
   <si>
@@ -222,16 +217,34 @@
   </si>
   <si>
     <t>14:12</t>
+  </si>
+  <si>
+    <t>18:05</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>10:53</t>
+  </si>
+  <si>
+    <t>Duration (min)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -582,250 +595,243 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63FD7E8-2180-5641-AFBE-A36407D78B6C}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView zoomScale="177" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" style="2" customWidth="1"/>
     <col min="5" max="7" width="10.83203125" style="2"/>
     <col min="9" max="9" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43905</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>1.86</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2">
-        <f>SUM(B:B)</f>
-        <v>34.800000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43918</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>2.92</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43919</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>3.06</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43921</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>3.03</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43923</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>3.05</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43925</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>1.81</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43927</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <v>1.98</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43932</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <v>2.89</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43939</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4">
         <v>2.0299999999999998</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43941</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="4">
         <v>2.2799999999999998</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="F11" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43942</v>
       </c>
@@ -833,56 +839,56 @@
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43948</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="4">
         <v>2.69</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43950</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="4">
         <v>1.53</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43953</v>
       </c>
@@ -890,44 +896,92 @@
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43953</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4">
         <v>1.1499999999999999</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43955</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4">
         <v>1.52</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>43958</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1.64</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>61</v>
+      <c r="E18" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>43967</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1.08</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34AD8D95-03AB-4346-9A7A-78B81C37127F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="186" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add exception handler and status updates
</commit_message>
<xml_diff>
--- a/running.xlsx
+++ b/running.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="16120" windowWidth="28800" xWindow="38620" yWindow="460"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="16120" windowWidth="28800" xWindow="38400" yWindow="460"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" state="visible" r:id="rId1"/>
@@ -382,8 +382,8 @@
     <col customWidth="1" max="7" min="5" style="1" width="10.83203125"/>
     <col customWidth="1" max="8" min="8" style="3" width="10.83203125"/>
     <col customWidth="1" max="9" min="9" style="3" width="16.33203125"/>
-    <col customWidth="1" max="16" min="10" style="3" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="17" style="3" width="10.83203125"/>
+    <col customWidth="1" max="20" min="10" style="3" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="21" style="3" width="10.83203125"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -787,10 +787,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0" zoomScale="186">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -799,8 +799,8 @@
     <col customWidth="1" max="2" min="2" style="4" width="13.1640625"/>
     <col customWidth="1" max="3" min="3" style="4" width="14.5"/>
     <col customWidth="1" max="4" min="4" style="4" width="12.6640625"/>
-    <col customWidth="1" max="10" min="5" style="4" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="11" style="4" width="10.83203125"/>
+    <col customWidth="1" max="14" min="5" style="4" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="15" style="4" width="10.83203125"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1246,17 +1246,105 @@
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>5/25/20</t>
         </is>
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t>1.65</t>
+          <t>2.99</t>
         </is>
       </c>
       <c r="C20" s="4" t="inlineStr">
         <is>
-          <t>30:32</t>
+          <t>40:42</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="inlineStr">
+        <is>
+          <t>13:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="C21" s="4" t="inlineStr">
+        <is>
+          <t>12:12</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="inlineStr">
+        <is>
+          <t>0:5</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>4/22/20</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>312</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="inlineStr">
+        <is>
+          <t>33123</t>
+        </is>
+      </c>
+      <c r="B23" s="4" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="C23" s="4" t="inlineStr">
+        <is>
+          <t>32:32</t>
+        </is>
+      </c>
+      <c r="D23" s="4" t="inlineStr">
+        <is>
+          <t>1:1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="inlineStr">
+        <is>
+          <t>05/26/2020</t>
+        </is>
+      </c>
+      <c r="B24" s="4" t="inlineStr">
+        <is>
+          <t>1.58</t>
+        </is>
+      </c>
+      <c r="C24" s="4" t="inlineStr">
+        <is>
+          <t>24:38</t>
+        </is>
+      </c>
+      <c r="D24" s="4" t="inlineStr">
+        <is>
+          <t>15:35</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add support for all data analysis functions
</commit_message>
<xml_diff>
--- a/running.xlsx
+++ b/running.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ishanshah/Documents/Programming/Projects/runkeeper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F46413-3E6F-C945-B49A-22EC9261D112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFDA340-AEE6-0348-98DC-EF1A93485023}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="1280" windowWidth="28800" windowHeight="16120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3460" yWindow="1280" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
-    <sheet name="test" sheetId="4" r:id="rId2"/>
+    <sheet name="test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -195,6 +195,18 @@
   </si>
   <si>
     <t>10:31</t>
+  </si>
+  <si>
+    <t>05/28/20</t>
+  </si>
+  <si>
+    <t>1.06</t>
+  </si>
+  <si>
+    <t>10:13</t>
+  </si>
+  <si>
+    <t>9:38</t>
   </si>
 </sst>
 </file>
@@ -230,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -239,6 +251,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,10 +569,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView zoomScale="177" workbookViewId="0">
-      <selection activeCell="D19" sqref="A1:D19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="177" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,8 +584,8 @@
     <col min="5" max="7" width="10.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="3" customWidth="1"/>
     <col min="9" max="9" width="16.33203125" style="3" customWidth="1"/>
-    <col min="10" max="23" width="10.83203125" style="3" customWidth="1"/>
-    <col min="24" max="16384" width="10.83203125" style="3"/>
+    <col min="10" max="29" width="10.83203125" style="3" customWidth="1"/>
+    <col min="30" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -841,6 +856,26 @@
       <c r="D19" s="1" t="s">
         <v>57</v>
       </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -849,11 +884,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938FA4C8-4AF2-924A-9009-62F55E91A5B6}">
-  <dimension ref="A1:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="183" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A4" zoomScale="183" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1129,6 +1164,12 @@
         <v>57</v>
       </c>
     </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>